<commit_message>
changes for boolean, chimera, ijpp
</commit_message>
<xml_diff>
--- a/contribs_boolean.xlsx
+++ b/contribs_boolean.xlsx
@@ -529,7 +529,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="8.86328125" customWidth="1" style="17" min="1" max="1"/>
     <col width="22.1328125" customWidth="1" style="17" min="2" max="2"/>
@@ -1646,7 +1646,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="8.86328125" customWidth="1" style="17" min="1" max="1"/>
     <col width="21.86328125" customWidth="1" style="17" min="2" max="2"/>
@@ -2694,7 +2694,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="24" customWidth="1" style="17" min="1" max="1"/>
     <col width="14.59765625" customWidth="1" style="17" min="2" max="2"/>
@@ -5808,7 +5808,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="26.1328125" customWidth="1" style="17" min="1" max="1"/>
     <col width="18.3984375" customWidth="1" style="17" min="2" max="2"/>
@@ -10615,7 +10615,7 @@
       <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="25" customWidth="1" style="17" min="1" max="1"/>
     <col width="24" customWidth="1" style="17" min="2" max="2"/>
@@ -14862,7 +14862,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="25.265625" customWidth="1" style="17" min="1" max="1"/>
     <col width="198.265625" customWidth="1" style="17" min="2" max="2"/>
@@ -17480,7 +17480,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="24" customWidth="1" style="17" min="1" max="1"/>
     <col width="8.86328125" customWidth="1" style="17" min="2" max="26"/>

</xml_diff>